<commit_message>
Updated to latest version
</commit_message>
<xml_diff>
--- a/ServiceInteractions/riv/insuranceprocess/healthreporting/trunk/docs/Tjanstekontrakt insuranceprocess healthreporting - Regler.xlsx
+++ b/ServiceInteractions/riv/insuranceprocess/healthreporting/trunk/docs/Tjanstekontrakt insuranceprocess healthreporting - Regler.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr checkCompatibility="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="18990" windowHeight="8610" activeTab="1"/>
+    <workbookView xWindow="10425" yWindow="-15" windowWidth="10500" windowHeight="10440"/>
   </bookViews>
   <sheets>
     <sheet name="Revisioner" sheetId="1" r:id="rId1"/>
@@ -129,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B43" authorId="0">
+    <comment ref="B46" authorId="0">
       <text>
         <r>
           <rPr>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="164">
   <si>
     <t>Version</t>
   </si>
@@ -250,30 +250,6 @@
     <t>Fält 5 - aktivitetsbegränsning</t>
   </si>
   <si>
-    <t>Fält 6 kryssruta 1 - given ordination</t>
-  </si>
-  <si>
-    <t>Fält 6 kryssruta 2 - fortsatt poliklinisk kontakt</t>
-  </si>
-  <si>
-    <t>Fält 6 kryssruta 3 - undvika belastning</t>
-  </si>
-  <si>
-    <t>Fält 6 kryssruta 4 - besöka arbetsplats</t>
-  </si>
-  <si>
-    <t>Fält 6 kryssruta 5 - väntar annan åtgärd sjukvården</t>
-  </si>
-  <si>
-    <t>Fält 6 kryssruta 6 - väntar annan åtgärd</t>
-  </si>
-  <si>
-    <t>Fält 6 kryssruta 7 - övrigt</t>
-  </si>
-  <si>
-    <t>O/V (1 till 7 av dessa kryssrutor måste väljas)</t>
-  </si>
-  <si>
     <t>Vid val skall även beskrivning anges</t>
   </si>
   <si>
@@ -283,24 +259,6 @@
     <t>Endast en av kryssrutorna skall anges</t>
   </si>
   <si>
-    <t>Fält 7, kryssrutor 4 - kontakt företagshälsovård</t>
-  </si>
-  <si>
-    <t>Fält 8 kryssruta 1-3 - arbete/arbetslöshet/föräldraledig</t>
-  </si>
-  <si>
-    <t>Fält 8 kryssruta 4 - nedsatt 1/4</t>
-  </si>
-  <si>
-    <t>Fält 8 kryssruta 5 - nedsatt hälften</t>
-  </si>
-  <si>
-    <t>Fält 8 kryssruta 6 - nedsatt 3/4</t>
-  </si>
-  <si>
-    <t>Fält 8 kryssruta 7 - nedsatt helt</t>
-  </si>
-  <si>
     <t>Båda datum skall anges samt datum t.o.m skall vara större än datum f.r.o.m.</t>
   </si>
   <si>
@@ -313,9 +271,6 @@
     <t>Fält 11, kryssruta 1-2 - resor till från arbetet</t>
   </si>
   <si>
-    <t>Fält 12, kryssruta 1-2 - kontakt med FK önskas</t>
-  </si>
-  <si>
     <t>Fält 13 - övriga upplysningar</t>
   </si>
   <si>
@@ -331,9 +286,6 @@
     <t>Fält 16 - läkarens namnteckning</t>
   </si>
   <si>
-    <t>Fält 17 - förskrivarkod och arbetsplatskod</t>
-  </si>
-  <si>
     <t>Obligatoriska/valbara fält samt fältregler</t>
   </si>
   <si>
@@ -341,39 +293,6 @@
   </si>
   <si>
     <t>Kommentarer</t>
-  </si>
-  <si>
-    <t>Används ej i piloten</t>
-  </si>
-  <si>
-    <t>VJ: Ej obligatorisk om Fält 1 är ifyllt?</t>
-  </si>
-  <si>
-    <t>HP: Ej obligatorisk om Fält 1 är ifyllt</t>
-  </si>
-  <si>
-    <t>VJ: Ej obligatorisk om Fält 1 är ifyllt?
-HP: Detta är det enda fältet av 2–8a som verkligen är tekniskt obligatoriskt om fält 1 inte är ifyllt. För alla andra fält finns undantag.</t>
-  </si>
-  <si>
-    <t>HP: V</t>
-  </si>
-  <si>
-    <t>HP: Fält 13 är inte tekniskt obligatoriskt om "Går ej att bedöma" är vald.</t>
-  </si>
-  <si>
-    <t>HP: Se kommentarer på 4 och 10, det bör diskuteras om detta verkligen ska styras så hårt iom att FK inte kräver det.</t>
-  </si>
-  <si>
-    <t>VJ: Ej obligatorisk om Fält 1 är ifyllt?
-HP: Fält 13 är inte tekniskt obligatoriskt om "annat" är ikryssat. Däremot stämmer det att man ska ange vad bedömningen baserats på om fält 1 inte är ifyllt. Funderar på om man inte borde kunna varna för om datum som sätts i fält 4 är &gt; dagens datum (man kan ju inte basera något på något som ännu inte hänt).</t>
-  </si>
-  <si>
-    <t>VJ: Ej obligatorisk om Fält 1 är ifyllt?
-HP: Beskrivningarna är inte tekniskt obligatoriska såsom anges i regelkolumnen.</t>
-  </si>
-  <si>
-    <t>AKA: Endast obligatoriskt om beslutsstödets rekommendation överskrids - dvs fel att det alltid måste anges.</t>
   </si>
   <si>
     <t>Struktur</t>
@@ -413,9 +332,6 @@
     <t>0:1</t>
   </si>
   <si>
-    <t>ersatterLakarutlatandeId</t>
-  </si>
-  <si>
     <t>person-id</t>
   </si>
   <si>
@@ -440,9 +356,6 @@
     <t>enhets-id</t>
   </si>
   <si>
-    <t>enhets-namn</t>
-  </si>
-  <si>
     <t>telefonnummer</t>
   </si>
   <si>
@@ -452,12 +365,6 @@
     <t>vardgivare-namn</t>
   </si>
   <si>
-    <t>signatur</t>
-  </si>
-  <si>
-    <t>signeringstidpunkt</t>
-  </si>
-  <si>
     <t>vardkontakttyp</t>
   </si>
   <si>
@@ -491,18 +398,12 @@
     <t>typAvArbetsuppgift</t>
   </si>
   <si>
-    <t>varaktighet</t>
-  </si>
-  <si>
     <t>nedsattningsgrad</t>
   </si>
   <si>
     <t>typAvSysselsattning</t>
   </si>
   <si>
-    <t>1:*</t>
-  </si>
-  <si>
     <t>0:2</t>
   </si>
   <si>
@@ -530,9 +431,6 @@
     <t>lakarutLatande.skapadAvHosPersonal.enhet.vardgivare</t>
   </si>
   <si>
-    <t>lakarutLatande.skapadAvHosPersonal.signatur</t>
-  </si>
-  <si>
     <t>lakarutLatande.vardkontakt</t>
   </si>
   <si>
@@ -569,24 +467,6 @@
     <t>Vardkontakttyp.MIN_TELEFONKONTAKT_MED_PATIENTEN</t>
   </si>
   <si>
-    <t>Aktivitetskod.GIVEN_ORDINATION</t>
-  </si>
-  <si>
-    <t>Aktivitetskod.FORTSATT_POLIKLINISK_KONTAKT</t>
-  </si>
-  <si>
-    <t>Aktivitetskod.UNDVIKA_VISS_BELASTNING</t>
-  </si>
-  <si>
-    <t>Aktivitetskod.BESOKA_ARBETSPLATSEN</t>
-  </si>
-  <si>
-    <t>Aktivitetskod.VANTAR_PA_ATGARD_INOM_SJUKVARDEN</t>
-  </si>
-  <si>
-    <t>Aktivitetskod.VANTAR_PA_ANNAN_ATGARD</t>
-  </si>
-  <si>
     <t>Aktivitetskod.OVRIGT</t>
   </si>
   <si>
@@ -629,9 +509,6 @@
     <t>Referenstyp.Annat</t>
   </si>
   <si>
-    <t>Endast en av kryssrutorna skall nages. Valbart om arbetslös fält 8 kryssruta 2. Om kryssruta 4 - Om Går ej att bedöma är vald skall även fält 13 fyllas i</t>
-  </si>
-  <si>
     <t>0.9</t>
   </si>
   <si>
@@ -656,16 +533,118 @@
     <t>DatumTid</t>
   </si>
   <si>
-    <t>DatumIntervall</t>
-  </si>
-  <si>
-    <t>Personnummer el. motsvarande</t>
-  </si>
-  <si>
     <t>HSA ID</t>
   </si>
   <si>
-    <t>MU7263-RIV_1.0.xsd</t>
+    <t>0.95</t>
+  </si>
+  <si>
+    <t>Anpassning för nya blanketten, samt uppdelning av MU7263</t>
+  </si>
+  <si>
+    <t>O*/V (1 till 4 av dessa kryssrutor måste väljas). Ej obligatoriskt om fält 1 ikryssat</t>
+  </si>
+  <si>
+    <t>O * Ej obligatoriskt om fält 1 ikryssat</t>
+  </si>
+  <si>
+    <t>Aktivitetskod.PATIENTEN_BEHOVER_FA_KONTAKT_MED_ARBETSFORMEDLINGEN</t>
+  </si>
+  <si>
+    <t>Fält 6a kryssruta 1 - kontakt med Arbetsförmedlingen</t>
+  </si>
+  <si>
+    <t>Fält 6a kryssruta 2 - kontakt med företagshälsovård</t>
+  </si>
+  <si>
+    <t>Fält 6a kryssruta 3 - Övrigt</t>
+  </si>
+  <si>
+    <t>Fält 6b kryssruta 1 - planerad eller pågående behandling eller åtgärd inom sjukvården</t>
+  </si>
+  <si>
+    <t>Fält 6b kryssruta 2 - planerad eller pågående behandling eller åtgärd - annan</t>
+  </si>
+  <si>
+    <t>O*/V (1 till 5 av dessa kryssrutor måste väljas). Ej obligatoriskt om fält 1 ikryssat</t>
+  </si>
+  <si>
+    <t>Aktivitetskod.PLANERAD_ELLER_PAGAENDE_BEHANDLING_ELLER_ATGARD_INOM_SJUKVARDEN</t>
+  </si>
+  <si>
+    <t>Aktivitetskod.PLANERAD_ELLER_PAGAENDE_ANNAN_ATGARD</t>
+  </si>
+  <si>
+    <t>Fält 8a kryssruta 1-3 - arbete/arbetslöshet/föräldraledig</t>
+  </si>
+  <si>
+    <t>Fält 8b kryssruta 1 - nedsatt 1/4</t>
+  </si>
+  <si>
+    <t>Fält 8b kryssruta 2 - nedsatt hälften</t>
+  </si>
+  <si>
+    <t>Fält 8b kryssruta 4 - nedsatt helt</t>
+  </si>
+  <si>
+    <t>Fält 8b kryssruta 3 - nedsatt 3/4</t>
+  </si>
+  <si>
+    <t>Endast en av kryssrutorna skall anges. Valbart om arbetslös fält 8a kryssruta 2. Om kryssruta 4 - Om Går ej att bedöma är vald skall även fält 13 fyllas i</t>
+  </si>
+  <si>
+    <t>Fält 17 - förskrivarkod</t>
+  </si>
+  <si>
+    <t>Fält 17 - arbetsplatskod</t>
+  </si>
+  <si>
+    <t>MU7263-RIV_2.0.xsd + Insuranceprocess_healthreporting_1.0.xsd</t>
+  </si>
+  <si>
+    <t>skickatdatum</t>
+  </si>
+  <si>
+    <t>signeringsdatum</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DDTHH:MM:ss</t>
+  </si>
+  <si>
+    <t>Personnummer el. samordningsnummer</t>
+  </si>
+  <si>
+    <t>forskrivarkod</t>
+  </si>
+  <si>
+    <t>arbetsplatskod</t>
+  </si>
+  <si>
+    <t>enhetsnamn</t>
+  </si>
+  <si>
+    <t>epost</t>
+  </si>
+  <si>
+    <t>varaktighetFrom</t>
+  </si>
+  <si>
+    <t>varaktighetTom</t>
+  </si>
+  <si>
+    <t>Fält 12, kryssruta 1- kontakt med FK önskas</t>
+  </si>
+  <si>
+    <t>Klinik eller mottagning - postort</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>Sista justering pga små ändringar i schemafilerna</t>
   </si>
 </sst>
 </file>
@@ -998,7 +977,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1128,6 +1107,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1454,8 +1439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1467,12 +1452,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -1504,7 +1489,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>158</v>
+        <v>118</v>
       </c>
       <c r="B4" s="6">
         <v>40303</v>
@@ -1513,20 +1498,36 @@
         <v>6</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>159</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
+      <c r="A5" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="6">
+        <v>40329</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
+      <c r="A6" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" s="6">
+        <v>40347</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="5"/>
@@ -1705,10 +1706,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P59"/>
+  <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1718,7 +1719,7 @@
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="257" max="257" width="81.42578125" customWidth="1"/>
     <col min="258" max="258" width="26" customWidth="1"/>
     <col min="262" max="262" width="9.85546875" customWidth="1"/>
@@ -2038,32 +2039,32 @@
   <sheetData>
     <row r="1" spans="1:16" s="30" customFormat="1" ht="27.75">
       <c r="A1" s="29" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="B1" s="29"/>
     </row>
     <row r="3" spans="1:16" s="31" customFormat="1" ht="15.75" thickBot="1"/>
     <row r="4" spans="1:16" s="31" customFormat="1" ht="38.25">
       <c r="A4" s="32" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="H4" s="33" t="s">
         <v>3</v>
@@ -2076,436 +2077,434 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="37" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D5" s="38"/>
       <c r="E5" s="38"/>
       <c r="F5" s="38"/>
       <c r="G5" s="39" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="H5" s="40" t="s">
-        <v>160</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="37" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D6" s="38"/>
       <c r="E6" s="38"/>
       <c r="F6" s="38"/>
       <c r="G6" s="39" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="H6" s="40"/>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="37" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="B7" s="41" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D7" s="38"/>
       <c r="E7" s="38"/>
       <c r="F7" s="38"/>
       <c r="G7" s="39" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="H7" s="40"/>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="37" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>85</v>
+        <v>150</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>161</v>
+        <v>1</v>
       </c>
       <c r="D8" s="38"/>
       <c r="E8" s="38"/>
       <c r="F8" s="38"/>
-      <c r="G8" s="39" t="s">
-        <v>84</v>
-      </c>
+      <c r="G8" s="39"/>
       <c r="H8" s="40" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="37" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="B9" s="41" t="s">
-        <v>86</v>
+        <v>149</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>161</v>
+        <v>125</v>
       </c>
       <c r="D9" s="38"/>
       <c r="E9" s="38"/>
       <c r="F9" s="38"/>
-      <c r="G9" s="39" t="s">
-        <v>80</v>
-      </c>
+      <c r="G9" s="39"/>
       <c r="H9" s="40" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="37" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
       <c r="B10" s="41" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D10" s="38"/>
       <c r="E10" s="38"/>
       <c r="F10" s="38"/>
       <c r="G10" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="H10" s="40"/>
+        <v>54</v>
+      </c>
+      <c r="H10" s="40" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="37" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
       <c r="B11" s="41" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D11" s="38"/>
       <c r="E11" s="38"/>
       <c r="F11" s="38"/>
       <c r="G11" s="39" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="H11" s="40"/>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="37" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D12" s="38"/>
       <c r="E12" s="38"/>
       <c r="F12" s="38"/>
       <c r="G12" s="39" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="H12" s="40"/>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="38" t="s">
         <v>121</v>
-      </c>
-      <c r="B13" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="C13" s="38" t="s">
-        <v>161</v>
       </c>
       <c r="D13" s="38"/>
       <c r="E13" s="38"/>
       <c r="F13" s="38"/>
       <c r="G13" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="H13" s="40" t="s">
-        <v>168</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="H13" s="40"/>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="38" t="s">
         <v>121</v>
-      </c>
-      <c r="B14" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="C14" s="38" t="s">
-        <v>161</v>
       </c>
       <c r="D14" s="38"/>
       <c r="E14" s="38"/>
       <c r="F14" s="38"/>
       <c r="G14" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="H14" s="40"/>
+        <v>54</v>
+      </c>
+      <c r="H14" s="40" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="37" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D15" s="38"/>
       <c r="E15" s="38"/>
       <c r="F15" s="38"/>
       <c r="G15" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="H15" s="40" t="s">
-        <v>168</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="H15" s="40"/>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="37" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>94</v>
+        <v>154</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D16" s="38"/>
       <c r="E16" s="38"/>
       <c r="F16" s="38"/>
       <c r="G16" s="39" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="H16" s="40"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="37" t="s">
-        <v>122</v>
+        <v>90</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>162</v>
+        <v>66</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D17" s="38"/>
       <c r="E17" s="38"/>
       <c r="F17" s="38"/>
       <c r="G17" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="H17" s="40"/>
+        <v>54</v>
+      </c>
+      <c r="H17" s="40" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="37" t="s">
-        <v>122</v>
+        <v>90</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D18" s="38"/>
       <c r="E18" s="38"/>
       <c r="F18" s="38"/>
       <c r="G18" s="39" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="H18" s="40"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="37" t="s">
-        <v>122</v>
+        <v>90</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D19" s="38"/>
       <c r="E19" s="38"/>
       <c r="F19" s="38"/>
       <c r="G19" s="39" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="H19" s="40"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="B20" s="41" t="s">
-        <v>95</v>
-      </c>
       <c r="C20" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D20" s="38"/>
       <c r="E20" s="38"/>
       <c r="F20" s="38"/>
       <c r="G20" s="39" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="H20" s="40"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="B21" s="41" t="s">
-        <v>96</v>
-      </c>
       <c r="C21" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D21" s="38"/>
       <c r="E21" s="38"/>
       <c r="F21" s="38"/>
       <c r="G21" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="H21" s="40" t="s">
-        <v>168</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="H21" s="40"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="37" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="B22" s="41" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D22" s="38"/>
       <c r="E22" s="38"/>
       <c r="F22" s="38"/>
       <c r="G22" s="39" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="H22" s="40"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="37" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="B23" s="41" t="s">
-        <v>98</v>
+        <v>157</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D23" s="38"/>
       <c r="E23" s="38"/>
       <c r="F23" s="38"/>
       <c r="G23" s="39" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="H23" s="40"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="37" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="B24" s="41" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>165</v>
+        <v>121</v>
       </c>
       <c r="D24" s="38"/>
       <c r="E24" s="38"/>
       <c r="F24" s="38"/>
       <c r="G24" s="39" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="H24" s="40"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="37" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="B25" s="41" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D25" s="38"/>
       <c r="E25" s="38"/>
       <c r="F25" s="38"/>
       <c r="G25" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="H25" s="40"/>
+        <v>54</v>
+      </c>
+      <c r="H25" s="40" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="37" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>166</v>
+        <v>121</v>
       </c>
       <c r="D26" s="38"/>
       <c r="E26" s="38"/>
       <c r="F26" s="38"/>
       <c r="G26" s="39" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="H26" s="40"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="37" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D27" s="38"/>
       <c r="E27" s="38"/>
       <c r="F27" s="38"/>
       <c r="G27" s="39" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="H27" s="40"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="37" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="B28" s="41" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="C28" s="38" t="s">
         <v>1</v>
@@ -2514,403 +2513,452 @@
       <c r="E28" s="38"/>
       <c r="F28" s="38"/>
       <c r="G28" s="39" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="H28" s="40"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="37" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="B29" s="41" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D29" s="38"/>
       <c r="E29" s="38"/>
       <c r="F29" s="38"/>
       <c r="G29" s="39" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="H29" s="40"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="37" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="C30" s="38" t="s">
-        <v>161</v>
+        <v>1</v>
       </c>
       <c r="D30" s="38"/>
       <c r="E30" s="38"/>
       <c r="F30" s="38"/>
       <c r="G30" s="39" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="H30" s="40"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="37" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="B31" s="41" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="C31" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D31" s="38"/>
       <c r="E31" s="38"/>
       <c r="F31" s="38"/>
       <c r="G31" s="39" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="H31" s="40"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="37" t="s">
-        <v>129</v>
+        <v>94</v>
       </c>
       <c r="B32" s="41" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="C32" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D32" s="38"/>
       <c r="E32" s="38"/>
       <c r="F32" s="38"/>
       <c r="G32" s="39" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="H32" s="40"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="37" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="C33" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D33" s="38"/>
       <c r="E33" s="38"/>
       <c r="F33" s="38"/>
       <c r="G33" s="39" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="H33" s="40"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="37" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="B34" s="41" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="C34" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D34" s="38"/>
       <c r="E34" s="38"/>
       <c r="F34" s="38"/>
       <c r="G34" s="39" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="H34" s="40"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="37" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="B35" s="41" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="C35" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D35" s="38"/>
       <c r="E35" s="38"/>
       <c r="F35" s="38"/>
       <c r="G35" s="39" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="H35" s="40"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="37" t="s">
-        <v>131</v>
+        <v>97</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="C36" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D36" s="38"/>
       <c r="E36" s="38"/>
       <c r="F36" s="38"/>
       <c r="G36" s="39" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="H36" s="40"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="37" t="s">
-        <v>131</v>
+        <v>97</v>
       </c>
       <c r="B37" s="41" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="C37" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D37" s="38"/>
       <c r="E37" s="38"/>
       <c r="F37" s="38"/>
       <c r="G37" s="39" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="H37" s="40"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="37" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="B38" s="41" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="C38" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D38" s="38"/>
       <c r="E38" s="38"/>
       <c r="F38" s="38"/>
       <c r="G38" s="39" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="H38" s="40"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="37" t="s">
-        <v>132</v>
+        <v>98</v>
       </c>
       <c r="B39" s="41" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="C39" s="38" t="s">
-        <v>166</v>
+        <v>121</v>
       </c>
       <c r="D39" s="38"/>
       <c r="E39" s="38"/>
       <c r="F39" s="38"/>
       <c r="G39" s="39" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="H39" s="40"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="37" t="s">
-        <v>132</v>
+        <v>86</v>
       </c>
       <c r="B40" s="41" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="C40" s="38" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D40" s="38"/>
       <c r="E40" s="38"/>
       <c r="F40" s="38"/>
       <c r="G40" s="39" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="H40" s="40"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="37" t="s">
-        <v>133</v>
-      </c>
-      <c r="B41" s="37" t="s">
-        <v>113</v>
+        <v>99</v>
+      </c>
+      <c r="B41" s="41" t="s">
+        <v>158</v>
       </c>
       <c r="C41" s="38" t="s">
-        <v>161</v>
+        <v>1</v>
       </c>
       <c r="D41" s="38"/>
       <c r="E41" s="38"/>
       <c r="F41" s="38"/>
       <c r="G41" s="39" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="H41" s="40"/>
     </row>
-    <row r="42" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A42" s="42"/>
-      <c r="B42" s="43"/>
-      <c r="C42" s="44"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44"/>
-      <c r="F42" s="44"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="46"/>
-    </row>
-    <row r="43" spans="1:8" ht="23.25" thickBot="1">
-      <c r="A43" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="B43" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="G43" s="45"/>
+    <row r="42" spans="1:8">
+      <c r="A42" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="C42" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="H42" s="40"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="B43" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="H43" s="40"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="37" t="s">
-        <v>119</v>
-      </c>
-      <c r="B44" s="39" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="37" t="s">
-        <v>120</v>
-      </c>
-      <c r="B45" s="39" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="B44" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="B46" s="39" t="s">
-        <v>80</v>
-      </c>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="H44" s="40"/>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A45" s="42"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="44"/>
+      <c r="D45" s="44"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="44"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="46"/>
+    </row>
+    <row r="46" spans="1:8" ht="23.25" thickBot="1">
+      <c r="A46" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="G46" s="45"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="37" t="s">
-        <v>122</v>
+        <v>87</v>
       </c>
       <c r="B47" s="39" t="s">
-        <v>114</v>
-      </c>
-      <c r="D47" s="49"/>
+        <v>54</v>
+      </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="37" t="s">
-        <v>123</v>
+        <v>88</v>
       </c>
       <c r="B48" s="39" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="37" t="s">
-        <v>124</v>
+        <v>89</v>
       </c>
       <c r="B49" s="39" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="37" t="s">
-        <v>125</v>
+        <v>90</v>
       </c>
       <c r="B50" s="39" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
+        <v>54</v>
+      </c>
+      <c r="D50" s="49"/>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="37" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="B51" s="39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" s="39" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="B53" s="39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>94</v>
+      </c>
+      <c r="B54" s="39" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="B55" s="39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="B56" s="39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57" s="39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="B58" s="39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="B59" s="39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="B60" s="39" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
-      <c r="A52" t="s">
-        <v>127</v>
-      </c>
-      <c r="B52" s="39" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="37" t="s">
-        <v>128</v>
-      </c>
-      <c r="B53" s="39" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="B54" s="39" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="37" t="s">
-        <v>130</v>
-      </c>
-      <c r="B55" s="39" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="37" t="s">
-        <v>131</v>
-      </c>
-      <c r="B56" s="39" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="B57" s="39" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="B58" s="39" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="37" t="s">
-        <v>133</v>
-      </c>
-      <c r="B59" s="39" t="s">
-        <v>117</v>
+    <row r="61" spans="1:4">
+      <c r="A61" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="B61" s="39" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2924,7 +2972,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="17" customFormat="1" ht="55.5">
       <c r="A1" s="17" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="19" customFormat="1" ht="20.25">
@@ -2935,13 +2983,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>153</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="22" customFormat="1">
@@ -2978,10 +3026,10 @@
       <c r="E5" s="21"/>
     </row>
     <row r="6" spans="1:9" s="22" customFormat="1">
-      <c r="A6" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="15" t="s">
+      <c r="A6" s="52" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6" s="52" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="20"/>
@@ -2990,7 +3038,7 @@
     </row>
     <row r="7" spans="1:9" s="22" customFormat="1">
       <c r="A7" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>19</v>
@@ -3001,10 +3049,10 @@
     </row>
     <row r="8" spans="1:9" s="22" customFormat="1">
       <c r="A8" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="B8" s="51" t="s">
+        <v>20</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="21"/>
@@ -3012,7 +3060,7 @@
     </row>
     <row r="9" spans="1:9" s="22" customFormat="1">
       <c r="A9" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>19</v>
@@ -3022,8 +3070,12 @@
       <c r="E9" s="21"/>
     </row>
     <row r="10" spans="1:9" s="22" customFormat="1">
-      <c r="A10" s="15"/>
-      <c r="B10" s="20"/>
+      <c r="A10" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>19</v>
+      </c>
       <c r="C10" s="20"/>
       <c r="D10" s="21"/>
       <c r="E10" s="21"/>
@@ -3038,33 +3090,29 @@
       <c r="C11" s="15"/>
       <c r="D11" s="28"/>
       <c r="E11" s="37" t="s">
-        <v>134</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="24" customFormat="1">
       <c r="A12" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="28" t="s">
-        <v>19</v>
+      <c r="B12" s="51" t="s">
+        <v>130</v>
       </c>
       <c r="C12" s="15"/>
-      <c r="D12" s="16" t="s">
-        <v>64</v>
-      </c>
+      <c r="D12" s="16"/>
       <c r="E12" s="37"/>
     </row>
-    <row r="13" spans="1:9" s="24" customFormat="1" ht="75">
+    <row r="13" spans="1:9" s="24" customFormat="1">
       <c r="A13" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>19</v>
+      <c r="B13" s="51" t="s">
+        <v>130</v>
       </c>
       <c r="C13" s="15"/>
-      <c r="D13" s="16" t="s">
-        <v>66</v>
-      </c>
+      <c r="D13" s="16"/>
       <c r="E13" s="37"/>
       <c r="F13" s="25"/>
       <c r="G13" s="26"/>
@@ -3075,434 +3123,366 @@
       <c r="A14" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>19</v>
+      <c r="B14" s="51" t="s">
+        <v>130</v>
       </c>
       <c r="C14" s="15"/>
-      <c r="D14" s="16" t="s">
-        <v>64</v>
-      </c>
+      <c r="D14" s="16"/>
       <c r="E14" s="37"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="15" t="s">
-        <v>19</v>
+      <c r="B15" s="51" t="s">
+        <v>130</v>
       </c>
       <c r="C15" s="15"/>
-      <c r="D15" s="16" t="s">
-        <v>64</v>
-      </c>
+      <c r="D15" s="16"/>
       <c r="E15" s="37"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="52" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="52" t="s">
+      <c r="B16" s="54" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="16" t="s">
-        <v>64</v>
-      </c>
+      <c r="D16" s="16"/>
       <c r="E16" s="37" t="s">
-        <v>135</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="52"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="16" t="s">
-        <v>64</v>
-      </c>
+      <c r="B17" s="54"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="16"/>
       <c r="E17" s="37" t="s">
-        <v>136</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="52"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="16" t="s">
-        <v>64</v>
-      </c>
+      <c r="B18" s="54"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="16"/>
       <c r="E18" s="37" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="165">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="52"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="16" t="s">
-        <v>70</v>
-      </c>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="16"/>
       <c r="E19" s="37" t="s">
-        <v>156</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>19</v>
+      <c r="B20" s="51" t="s">
+        <v>130</v>
       </c>
       <c r="C20" s="15"/>
-      <c r="D20" s="16" t="s">
-        <v>64</v>
-      </c>
+      <c r="D20" s="16"/>
       <c r="E20" s="37"/>
     </row>
-    <row r="21" spans="1:5" ht="60">
-      <c r="A21" s="15" t="s">
+    <row r="21" spans="1:5">
+      <c r="A21" s="51" t="s">
+        <v>132</v>
+      </c>
+      <c r="B21" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="37" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="51" t="s">
+        <v>133</v>
+      </c>
+      <c r="B22" s="54"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="37" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="51" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" s="54"/>
+      <c r="C23" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="52" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" s="37" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="15" t="s">
+      <c r="D23" s="16"/>
+      <c r="E23" s="37" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30">
+      <c r="A24" s="51" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24" s="54"/>
+      <c r="C24" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="16"/>
+      <c r="E24" s="37" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30">
+      <c r="A25" s="51" t="s">
+        <v>136</v>
+      </c>
+      <c r="B25" s="54"/>
+      <c r="C25" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="16"/>
+      <c r="E25" s="37" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="45">
+      <c r="A26" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="52"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E22" s="37" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="15" t="s">
+      <c r="B26" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="C26" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="52"/>
-      <c r="C23" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E23" s="37" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="15" t="s">
+      <c r="D26" s="16"/>
+      <c r="E26" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30">
+      <c r="A27" s="51" t="s">
+        <v>140</v>
+      </c>
+      <c r="B27" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30">
+      <c r="A28" s="51" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="52"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E24" s="37" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="52"/>
-      <c r="C25" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" s="37" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="52"/>
-      <c r="C26" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" s="37" t="s">
+      <c r="D28" s="28"/>
+      <c r="E28" s="37" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30">
+      <c r="A29" s="51" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="52"/>
-      <c r="C27" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E27" s="37" t="s">
+      <c r="B29" s="54"/>
+      <c r="C29" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="28"/>
+      <c r="E29" s="37" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30">
+      <c r="A30" s="51" t="s">
+        <v>144</v>
+      </c>
+      <c r="B30" s="54"/>
+      <c r="C30" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="28"/>
+      <c r="E30" s="37" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="30">
+      <c r="A31" s="51" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="45">
-      <c r="A28" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E28" s="28" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E29" s="37" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30">
-      <c r="A30" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" s="28" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30">
-      <c r="A31" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" s="52" t="s">
-        <v>29</v>
-      </c>
+      <c r="B31" s="54"/>
       <c r="C31" s="15" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D31" s="28"/>
       <c r="E31" s="37" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="15"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+    </row>
+    <row r="33" spans="1:6" ht="45">
+      <c r="A33" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="51" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="30">
-      <c r="A32" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" s="52"/>
-      <c r="C32" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D32" s="28"/>
-      <c r="E32" s="37" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="30">
-      <c r="A33" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" s="52"/>
-      <c r="C33" s="15" t="s">
-        <v>49</v>
-      </c>
       <c r="D33" s="28"/>
-      <c r="E33" s="37" t="s">
-        <v>147</v>
+      <c r="E33" s="28" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="30">
       <c r="A34" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="52"/>
-      <c r="C34" s="15" t="s">
-        <v>49</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B34" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="15"/>
       <c r="D34" s="28"/>
-      <c r="E34" s="37" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="60">
-      <c r="A35" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B35" s="15" t="s">
+      <c r="E34" s="28" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="30">
+      <c r="A35" s="51" t="s">
+        <v>160</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="15"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="15"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="37"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="E35" s="28"/>
-    </row>
-    <row r="36" spans="1:6" ht="45">
-      <c r="A36" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36" s="28" t="s">
+      <c r="C37" s="15"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="15"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="37"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="27"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="B40" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="27"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="37"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="B41" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="28" t="s">
-        <v>157</v>
-      </c>
-      <c r="D36" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="E36" s="28" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="30">
-      <c r="A37" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B37" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="E37" s="28" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="30">
-      <c r="A38" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38" s="15"/>
-      <c r="D38" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="E38" s="28" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="60">
-      <c r="A39" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C39" s="15"/>
-      <c r="D39" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="E39" s="37"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C40" s="15"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="28"/>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="28" t="s">
-        <v>63</v>
-      </c>
+      <c r="C41" s="27"/>
+      <c r="D41" s="51"/>
       <c r="E41" s="37"/>
     </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="B42" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C42" s="27"/>
-      <c r="D42" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="E42" s="28"/>
-    </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="B43" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C43" s="27"/>
-      <c r="D43" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="E43" s="37"/>
+      <c r="D43" s="50"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="50"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="D44" s="50"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="50"/>
     </row>
     <row r="45" spans="1:6">
       <c r="D45" s="50"/>
-      <c r="E45" s="43"/>
+      <c r="E45" s="50"/>
       <c r="F45" s="50"/>
     </row>
     <row r="46" spans="1:6">
       <c r="D46" s="50"/>
-      <c r="E46" s="43"/>
+      <c r="E46" s="50"/>
       <c r="F46" s="50"/>
     </row>
     <row r="47" spans="1:6">
@@ -3512,22 +3492,22 @@
     </row>
     <row r="48" spans="1:6">
       <c r="D48" s="50"/>
-      <c r="E48" s="50"/>
+      <c r="E48" s="43"/>
       <c r="F48" s="50"/>
     </row>
     <row r="49" spans="4:6">
       <c r="D49" s="50"/>
-      <c r="E49" s="50"/>
+      <c r="E49" s="43"/>
       <c r="F49" s="50"/>
     </row>
     <row r="50" spans="4:6">
       <c r="D50" s="50"/>
-      <c r="E50" s="43"/>
+      <c r="E50" s="50"/>
       <c r="F50" s="50"/>
     </row>
     <row r="51" spans="4:6">
       <c r="D51" s="50"/>
-      <c r="E51" s="43"/>
+      <c r="E51" s="50"/>
       <c r="F51" s="50"/>
     </row>
     <row r="52" spans="4:6">
@@ -3550,22 +3530,12 @@
       <c r="E55" s="50"/>
       <c r="F55" s="50"/>
     </row>
-    <row r="56" spans="4:6">
-      <c r="D56" s="50"/>
-      <c r="E56" s="50"/>
-      <c r="F56" s="50"/>
-    </row>
-    <row r="57" spans="4:6">
-      <c r="D57" s="50"/>
-      <c r="E57" s="50"/>
-      <c r="F57" s="50"/>
-    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C16:C19"/>
     <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B21:B27"/>
-    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="B28:B31"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed motivering to optional
</commit_message>
<xml_diff>
--- a/ServiceInteractions/riv/insuranceprocess/healthreporting/trunk/docs/Tjanstekontrakt insuranceprocess healthreporting - Regler.xlsx
+++ b/ServiceInteractions/riv/insuranceprocess/healthreporting/trunk/docs/Tjanstekontrakt insuranceprocess healthreporting - Regler.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr checkCompatibility="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10425" yWindow="-15" windowWidth="10500" windowHeight="10440"/>
+    <workbookView xWindow="10425" yWindow="-15" windowWidth="10500" windowHeight="10440" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Revisioner" sheetId="1" r:id="rId1"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="165">
   <si>
     <t>Version</t>
   </si>
@@ -645,6 +645,9 @@
   </si>
   <si>
     <t>Sista justering pga små ändringar i schemafilerna</t>
+  </si>
+  <si>
+    <t>Minst en kryssruta skall anges</t>
   </si>
 </sst>
 </file>
@@ -977,7 +980,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1107,6 +1110,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1439,7 +1445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1452,12 +1458,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -2956,8 +2962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3145,10 +3151,10 @@
       <c r="A16" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="55" t="s">
         <v>129</v>
       </c>
-      <c r="C16" s="54" t="s">
+      <c r="C16" s="55" t="s">
         <v>30</v>
       </c>
       <c r="D16" s="16"/>
@@ -3160,8 +3166,8 @@
       <c r="A17" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="54"/>
-      <c r="C17" s="54"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
       <c r="D17" s="16"/>
       <c r="E17" s="37" t="s">
         <v>103</v>
@@ -3171,8 +3177,8 @@
       <c r="A18" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="54"/>
-      <c r="C18" s="54"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="55"/>
       <c r="D18" s="16"/>
       <c r="E18" s="37" t="s">
         <v>116</v>
@@ -3182,8 +3188,8 @@
       <c r="A19" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="55"/>
       <c r="D19" s="16"/>
       <c r="E19" s="37" t="s">
         <v>117</v>
@@ -3204,7 +3210,7 @@
       <c r="A21" s="51" t="s">
         <v>132</v>
       </c>
-      <c r="B21" s="54" t="s">
+      <c r="B21" s="55" t="s">
         <v>137</v>
       </c>
       <c r="C21" s="15"/>
@@ -3217,7 +3223,7 @@
       <c r="A22" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="B22" s="54"/>
+      <c r="B22" s="55"/>
       <c r="C22" s="15"/>
       <c r="D22" s="16"/>
       <c r="E22" s="37" t="s">
@@ -3228,7 +3234,7 @@
       <c r="A23" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="B23" s="54"/>
+      <c r="B23" s="55"/>
       <c r="C23" s="15" t="s">
         <v>32</v>
       </c>
@@ -3241,7 +3247,7 @@
       <c r="A24" s="51" t="s">
         <v>135</v>
       </c>
-      <c r="B24" s="54"/>
+      <c r="B24" s="55"/>
       <c r="C24" s="51" t="s">
         <v>32</v>
       </c>
@@ -3254,7 +3260,7 @@
       <c r="A25" s="51" t="s">
         <v>136</v>
       </c>
-      <c r="B25" s="54"/>
+      <c r="B25" s="55"/>
       <c r="C25" s="15" t="s">
         <v>32</v>
       </c>
@@ -3285,8 +3291,8 @@
       <c r="B27" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="C27" s="15" t="s">
-        <v>34</v>
+      <c r="C27" s="53" t="s">
+        <v>164</v>
       </c>
       <c r="D27" s="28"/>
       <c r="E27" s="28" t="s">
@@ -3297,7 +3303,7 @@
       <c r="A28" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="B28" s="54" t="s">
+      <c r="B28" s="55" t="s">
         <v>29</v>
       </c>
       <c r="C28" s="15" t="s">
@@ -3312,7 +3318,7 @@
       <c r="A29" s="51" t="s">
         <v>142</v>
       </c>
-      <c r="B29" s="54"/>
+      <c r="B29" s="55"/>
       <c r="C29" s="15" t="s">
         <v>35</v>
       </c>
@@ -3325,7 +3331,7 @@
       <c r="A30" s="51" t="s">
         <v>144</v>
       </c>
-      <c r="B30" s="54"/>
+      <c r="B30" s="55"/>
       <c r="C30" s="15" t="s">
         <v>35</v>
       </c>
@@ -3338,7 +3344,7 @@
       <c r="A31" s="51" t="s">
         <v>143</v>
       </c>
-      <c r="B31" s="54"/>
+      <c r="B31" s="55"/>
       <c r="C31" s="15" t="s">
         <v>35</v>
       </c>
@@ -3351,8 +3357,8 @@
       <c r="A32" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="15" t="s">
-        <v>19</v>
+      <c r="B32" s="53" t="s">
+        <v>20</v>
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="28"/>

</xml_diff>